<commit_message>
Better handle organizations and blank lines
</commit_message>
<xml_diff>
--- a/TCCON_Metadata_Template.xlsx
+++ b/TCCON_Metadata_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tmorrell/Documents/TCCON/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tmorrell/Documents/manage_dois/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52CBAD8A-A34E-3544-9216-B2BB2D6EF16A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5CCB1DF-14CC-864E-A39F-CB4E137799AB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33300" yWindow="1860" windowWidth="31260" windowHeight="12800" tabRatio="308" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4700" yWindow="4600" windowWidth="31260" windowHeight="12800" tabRatio="308" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="site" sheetId="5" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="64">
   <si>
     <t>family name</t>
   </si>
@@ -57,9 +57,6 @@
   </si>
   <si>
     <t>contributor type</t>
-  </si>
-  <si>
-    <t>Other</t>
   </si>
   <si>
     <t>Instructions:
@@ -150,25 +147,16 @@
     <t>DP160101598</t>
   </si>
   <si>
-    <t>Lopez</t>
-  </si>
-  <si>
     <t>Morino</t>
   </si>
   <si>
     <t>Isamu</t>
   </si>
   <si>
-    <t>Oscar M.</t>
-  </si>
-  <si>
     <t>National Institute for Environmental Studies</t>
   </si>
   <si>
     <t>National Institute for Environmental Studies (NIES), Onogawa 16-2, Tsukuba, Ibaraki 305-8506 (JP)</t>
-  </si>
-  <si>
-    <t>First Philipine Holdings (PH)</t>
   </si>
   <si>
     <t xml:space="preserve">0000-0003-2720-1569 </t>
@@ -236,12 +224,54 @@
   <si>
     <t>10.5194/amt-10-2627-2017</t>
   </si>
+  <si>
+    <t>HostingInstitution</t>
+  </si>
+  <si>
+    <t>California Institute of Techonolgy</t>
+  </si>
+  <si>
+    <t>DataCurator</t>
+  </si>
+  <si>
+    <t>Roehl</t>
+  </si>
+  <si>
+    <t>C. M.</t>
+  </si>
+  <si>
+    <t>California Institute of Techonolgy, Pasadena, CA (US)</t>
+  </si>
+  <si>
+    <t>0000-0001-5383-8462</t>
+  </si>
+  <si>
+    <t>ResearchGroup</t>
+  </si>
+  <si>
+    <t>TCCON</t>
+  </si>
+  <si>
+    <t>ContactPerson</t>
+  </si>
+  <si>
+    <t>Pollard</t>
+  </si>
+  <si>
+    <t>Dave</t>
+  </si>
+  <si>
+    <t>National Institute of Water and Atmospheric Research Ltd (NIWA), Lauder (NZ) </t>
+  </si>
+  <si>
+    <t>0000-0001-9923-2984</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -264,6 +294,12 @@
       <u/>
       <sz val="10"/>
       <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -310,7 +346,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -323,10 +359,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -725,7 +762,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="15" customWidth="1"/>
+    <col min="1" max="1" width="23.5" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="14.6640625" customWidth="1"/>
     <col min="4" max="5" width="15.83203125" customWidth="1"/>
     <col min="6" max="6" width="18.6640625" customWidth="1"/>
@@ -733,47 +771,47 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="4" spans="1:8" ht="107" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
+      <c r="A4" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
     </row>
     <row r="23" ht="13" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="29" ht="13" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -822,36 +860,36 @@
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>36</v>
-      </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
         <v>24</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
         <v>25</v>
       </c>
-      <c r="C3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>26</v>
-      </c>
-      <c r="E3" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
@@ -861,15 +899,15 @@
       <c r="C5" s="5"/>
     </row>
     <row r="23" spans="1:7" ht="113.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
@@ -925,27 +963,54 @@
     </row>
     <row r="2" spans="1:253" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:253" x14ac:dyDescent="0.15">
-      <c r="A3" s="3"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:253" ht="14" x14ac:dyDescent="0.15">
+      <c r="A3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="4" spans="1:253" x14ac:dyDescent="0.15">
-      <c r="A4" s="3"/>
+      <c r="A4" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="3"/>
     </row>
     <row r="5" spans="1:253" x14ac:dyDescent="0.15">
-      <c r="A5" s="3"/>
-      <c r="E5" s="3"/>
+      <c r="A5" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E5" t="s">
+        <v>63</v>
+      </c>
       <c r="I5" s="3"/>
       <c r="M5" s="3"/>
       <c r="Q5" s="3"/>
@@ -1070,23 +1135,27 @@
       <c r="A25" s="3"/>
     </row>
     <row r="27" spans="1:6" ht="124.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
+      <c r="A27" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="1">
     <mergeCell ref="A27:F27"/>
   </mergeCells>
-  <dataValidations count="1">
-    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="IS5 E5 I5 M5 Q5 U5 Y5 AC5 AG5 AK5 AO5 AS5 AW5 BA5 BE5 BI5 BM5 BQ5 BU5 BY5 CC5 CG5 CK5 CO5 CS5 CW5 DA5 DE5 DI5 DM5 DQ5 DU5 DY5 EC5 EG5 EK5 EO5 ES5 EW5 FA5 FE5 FI5 FM5 FQ5 FU5 FY5 GC5 GG5 GK5 GO5 GS5 GW5 HA5 HE5 HI5 HM5 HQ5 HU5 HY5 IC5 IG5 IK5 IO5 A2:A25" xr:uid="{00000000-0002-0000-0200-000000000000}">
+  <dataValidations count="2">
+    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="IS5 A2:A25 I5 M5 Q5 U5 Y5 AC5 AG5 AK5 AO5 AS5 AW5 BA5 BE5 BI5 BM5 BQ5 BU5 BY5 CC5 CG5 CK5 CO5 CS5 CW5 DA5 DE5 DI5 DM5 DQ5 DU5 DY5 EC5 EG5 EK5 EO5 ES5 EW5 FA5 FE5 FI5 FM5 FQ5 FU5 FY5 GC5 GG5 GK5 GO5 GS5 GW5 HA5 HE5 HI5 HM5 HQ5 HU5 HY5 IC5 IG5 IK5 IO5" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"ContactPerson,DataCollector,DataCurator,DataManager,Distributor,Editor,HostingInstitution,Producer,ProjectLeader,ProjectManager,ProjectMember,RegistrationAgency,RegistrationAuthority,RelatedPerson,Researcher,ResearchGroup,RightsHolder"</formula1>
+    </dataValidation>
+    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="E4" xr:uid="{1AB66D00-5E5B-0640-8014-AD6CA09B330E}">
+      <formula1>"ContactPerson  ,DataCollector ,DataCurator  ,DataManager  ,Distributor ,Editor ,HostingInstitution ,Producer ,ProjectLeader ,ProjectManager ,ProjectMember ,RegistrationAgency ,RegistrationAuthority ,RelatedPerson ,Researcher ,ResearchGroup ,RightsHolder ,"</formula1>
+      <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -1115,201 +1184,198 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>53</v>
+        <v>12</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A15" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A21" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B21" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" s="4" customFormat="1" ht="62" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" s="4" customFormat="1" ht="62" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="1">
     <mergeCell ref="A25:D25"/>
   </mergeCells>
-  <dataValidations count="3">
-    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="B3:B21" xr:uid="{00000000-0002-0000-0300-000000000000}">
+  <dataValidations count="2">
+    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="B2:B21" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>"ARK,arXiv,bibcode,DOI,EAN13,EISSN,Handle,IGSN,ISBN,ISSN,ISTC,LISSN,LSID,PMID,PURL,UPC,URL,URN"</formula1>
     </dataValidation>
     <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="A2:A21" xr:uid="{00000000-0002-0000-0300-000001000000}">
       <formula1>"IsCitedBy,Cites,IsSupplementTo,IsSupplementedBy,IsContinuedBy,Continues,HasMetadata,IsMetadataFor,IsNewVersionOf,IsPreviousVersionOf,IsPartOf,HasPart,IsReferencedBy,References,IsDocumentedBy,Documents,IsCompiledBy,Compiles,IsVariantFormOf,IsOriginalFormOf"</formula1>
       <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="B2" xr:uid="{35F295FB-41C5-724F-9E63-13833BBF02D5}">
-      <formula1>"ARK,arXiv,bibcode,DOI,EAN13,EISSN,Handle,IGSN,ISBN,ISSN,ISTC,LISSN,LSID,PMID,PURL,UPC,URL,URN"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -1339,33 +1405,33 @@
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -1373,27 +1439,27 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>29</v>
-      </c>
-      <c r="D4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
@@ -1406,14 +1472,14 @@
       <c r="B7" s="3"/>
     </row>
     <row r="13" spans="1:6" ht="80" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
+      <c r="A13" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>

</xml_diff>